<commit_message>
fixing test spreadsheets format
</commit_message>
<xml_diff>
--- a/regionalizacao/tests/data/test_DistritoZonaFromToSpreadsheet.xlsx
+++ b/regionalizacao/tests/data/test_DistritoZonaFromToSpreadsheet.xlsx
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">coddist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distrito</t>
   </si>
   <si>
     <t xml:space="preserve">zona</t>
@@ -34,16 +31,10 @@
     <t xml:space="preserve">01</t>
   </si>
   <si>
-    <t xml:space="preserve">AGUA RASA</t>
-  </si>
-  <si>
     <t xml:space="preserve">LESTE</t>
   </si>
   <si>
     <t xml:space="preserve">02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALTO DE PINHEIROS</t>
   </si>
   <si>
     <t xml:space="preserve">OESTE</t>
@@ -61,6 +52,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -126,12 +118,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -160,10 +148,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -178,31 +166,25 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="AMJ3" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>